<commit_message>
added logic to wait for downloads
The program will now check and wait for any chrome downloads to finish before closing the browser, in the event the download has not yet completed.
</commit_message>
<xml_diff>
--- a/BCS_template.xlsx
+++ b/BCS_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\ProgramingProjects\vc_extract_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\driggerst\Python\vc_extract_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF88589-F9EF-41A8-B31A-C09CA68D9837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38910" yWindow="4035" windowWidth="27945" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="New Vendors" sheetId="1" r:id="rId1"/>
@@ -86,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -445,11 +444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -530,7 +529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -561,10 +560,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73279012-FA0D-4144-9747-B9FB1AB2525D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>